<commit_message>
:fire: add batch job flow
</commit_message>
<xml_diff>
--- a/batch/src/test/resources/customerRawDto.xlsx
+++ b/batch/src/test/resources/customerRawDto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\learn\spring-boot-example\batch\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17E65D9-D2FF-4809-8325-ECCBAE831C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A64D5FE-CF77-49D5-9F53-B7395FB29E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="5190" windowWidth="38700" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="4350" windowWidth="38700" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,7 +416,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -448,6 +448,9 @@
         <f>"iphone"</f>
         <v>iphone</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="D2" t="str">
         <f>"150"</f>
         <v>150</v>

</xml_diff>